<commit_message>
added beta release note
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/FashionValley_two_conc_bad_measure_data.xlsx
+++ b/tests/testthat/test_data/FashionValley_two_conc_bad_measure_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/PartTimers/Nick Lombardo/BMP/FWCCalculator/tests/testthat/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{68B12495-BDB8-4764-870B-A0DD9101E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AF9FD59-8F7A-4D23-8279-625FB6AE8379}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{68B12495-BDB8-4764-870B-A0DD9101E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD8EF960-94D2-4815-ADE3-4F5CFAD145BF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Sample Time</t>
   </si>
@@ -68,12 +68,6 @@
   </si>
   <si>
     <t>"something"</t>
-  </si>
-  <si>
-    <t>"25.5"</t>
-  </si>
-  <si>
-    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -144,6 +138,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1717AE6F-0ADB-43C7-978E-616F04EDE151}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -423,7 +421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B646"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -755,8 +755,8 @@
       <c r="A41" s="1">
         <v>44264.406249999905</v>
       </c>
-      <c r="B41" t="s">
-        <v>11</v>
+      <c r="B41">
+        <v>26.3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,8 +875,8 @@
       <c r="A56" s="1">
         <v>44264.562499999869</v>
       </c>
-      <c r="B56" t="s">
-        <v>10</v>
+      <c r="B56">
+        <v>26.3</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -5901,30 +5901,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -5951,6 +5929,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6039,6 +6018,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -6182,7 +6166,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{573478D7-CB3C-4F77-932A-DAE8407B2792}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{851FA841-BED3-4AA9-8CA6-6B5F6DAC2D17}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D782A14-F801-4D81-AC35-0B683C77D4CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6194,32 +6212,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{851FA841-BED3-4AA9-8CA6-6B5F6DAC2D17}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29B58E0D-20BE-4A84-9419-20FAFBF18F8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
-    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>